<commit_message>
Add mechanical build guide and correct BOM omissions
</commit_message>
<xml_diff>
--- a/hardware/BOM/Planetary_Bean_Bouncer_BOM.xlsx
+++ b/hardware/BOM/Planetary_Bean_Bouncer_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t>Planetary Bean Bouncer BOM</t>
   </si>
@@ -28,9 +28,6 @@
     <t>8 Cup SS Flour Sifter</t>
   </si>
   <si>
-    <t>2040 V-Groove Extrusion Pre-cut lengths 300mm-2000mm - ZYLtech Engineering, LLC</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/DAOKI-Expansion-Arduino-Heatsink-Engraving/dp/B08KFYKKN4</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>https://www.amazon.com/%EF%BC%BB12-Pack%EF%BC%BD625-2RS-Ball-Bearings-Miniature/dp/B0BRQP2QG7?th=1</t>
   </si>
   <si>
-    <t>625-2RS bearings (12 pack) (planet bearings only 6 needed)</t>
-  </si>
-  <si>
     <t>https://boltdepot.com/Product-Details?product=6633</t>
   </si>
   <si>
@@ -266,6 +260,30 @@
   </si>
   <si>
     <t>See Sweet Maria’s wobble disc fabrication guide (link in README).</t>
+  </si>
+  <si>
+    <t>https://www.zyltech.com/2040-v-groove-extrusion-pre-cut-lengths-300mm-2000mm/</t>
+  </si>
+  <si>
+    <t>https://www.zyltech.com/high-accuracy-0-9-step-angle-nema-17-stepper-motor-1-5-a-0-42-nm-59-ozin/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.9 Step Angle Nema 17 Stepper Motor 1.5 A</t>
+  </si>
+  <si>
+    <t>https://www.zyltech.com/flexible-rubber-extrusion-strips-for-20mm-aluminum-extrustion-black-blue-or-white/</t>
+  </si>
+  <si>
+    <t>Flexible Rubber Extrusion Strips (10 meters)</t>
+  </si>
+  <si>
+    <t>Keeps most of Chaff from roasting out of extrusions</t>
+  </si>
+  <si>
+    <t>625-2RS bearings (12 pack) (planet bearings only 7 needed)</t>
+  </si>
+  <si>
+    <t>1 bearing end of shaft rides on.</t>
   </si>
 </sst>
 </file>
@@ -668,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,25 +707,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -722,7 +740,7 @@
         <v>28.99</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G11" si="0">B3*F3</f>
+        <f t="shared" ref="G3:G13" si="0">B3*F3</f>
         <v>28.99</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -744,7 +762,7 @@
         <v>23.99</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,7 +770,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="2">
         <v>10.08</v>
@@ -762,7 +780,7 @@
         <v>40.32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -770,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2">
         <v>6.95</v>
@@ -780,7 +798,7 @@
         <v>6.95</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -788,17 +806,20 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
       </c>
       <c r="F7" s="2">
-        <v>8.99</v>
+        <v>11.95</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="0"/>
-        <v>8.99</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>72</v>
+        <v>11.95</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,17 +827,17 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2">
-        <v>18.989999999999998</v>
+        <v>8.99</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>18.989999999999998</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>5</v>
+        <v>8.99</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,17 +845,17 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2">
-        <v>3.99</v>
+        <v>12.95</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>3.99</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
+        <v>12.95</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -842,17 +863,17 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2">
-        <v>7.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>7.99</v>
+        <v>18.989999999999998</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -860,161 +881,161 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2">
-        <v>7.99</v>
+        <v>3.99</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>7.99</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>68</v>
+        <v>3.99</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2">
-        <v>0.12</v>
+        <v>7.99</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" ref="G12:G20" si="1">B12*F12</f>
-        <v>0.48</v>
+        <f t="shared" si="0"/>
+        <v>7.99</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.99</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" ref="G14:G22" si="1">B14*F14</f>
+        <v>0.48</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2">
         <v>0.08</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G15" s="2">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="F16" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G16" s="2">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="H16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="2">
         <v>8.6</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G17" s="2">
         <f t="shared" si="1"/>
         <v>8.6</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="F18" s="2">
         <v>7.95</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G18" s="2">
         <f t="shared" si="1"/>
         <v>7.95</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="H18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
         <v>0.24</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G19" s="2">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.32</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.96</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="2">
-        <v>8.99</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="1"/>
-        <v>8.99</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1022,113 +1043,128 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F20" s="2">
-        <v>0.05</v>
+        <v>0.32</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>0.15000000000000002</v>
+        <v>0.96</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H21" s="1"/>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>8.99</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2">
         <v>0.09</v>
       </c>
-      <c r="G22" s="2">
-        <f>B22*F22</f>
+      <c r="G24" s="2">
+        <f>B24*F24</f>
         <v>0.72</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23">
+      <c r="H24" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G23" s="2">
-        <f>B23*F23</f>
+      <c r="G25" s="2">
+        <f>B25*F25</f>
         <v>1.6800000000000002</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="H25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="E28" s="5"/>
+      <c r="F28" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="G28" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="10" t="s">
+      <c r="H28" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="3">
-        <v>55</v>
-      </c>
-      <c r="G27" s="2">
-        <f>B27*F27</f>
-        <v>55</v>
-      </c>
-      <c r="H27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
@@ -1137,119 +1173,101 @@
       <c r="C29" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="2">
-        <v>7.99</v>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="3">
+        <v>55</v>
       </c>
       <c r="G29" s="2">
         <f>B29*F29</f>
-        <v>7.99</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="G30" s="2">
-        <f>B30*F30</f>
-        <v>0.12</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F31" s="2">
-        <v>0.22</v>
+        <v>7.99</v>
       </c>
       <c r="G31" s="2">
         <f>B31*F31</f>
-        <v>0.88</v>
+        <v>7.99</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F32" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="G32" s="2">
         <f>B32*F32</f>
-        <v>0.28000000000000003</v>
+        <v>0.12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>35</v>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="G33" s="2">
+        <f>B33*F33</f>
+        <v>0.88</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F34" s="2">
-        <v>9.69</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G34" s="2">
         <f>B34*F34</f>
-        <v>9.69</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
-      </c>
       <c r="D35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="2">
-        <v>7.88</v>
-      </c>
-      <c r="G35" s="2">
-        <f>B35*F35</f>
-        <v>7.88</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1257,146 +1275,190 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F36" s="2">
-        <v>7.99</v>
+        <v>9.69</v>
       </c>
       <c r="G36" s="2">
         <f>B36*F36</f>
-        <v>7.99</v>
+        <v>9.69</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F37" s="2">
-        <v>0.19</v>
+        <v>7.88</v>
       </c>
       <c r="G37" s="2">
         <f>B37*F37</f>
-        <v>0.38</v>
+        <v>7.88</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
       <c r="D38" t="s">
-        <v>50</v>
-      </c>
-      <c r="H38" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="F38" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="G38" s="2">
+        <f>B38*F38</f>
+        <v>7.99</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
       <c r="D39" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="1"/>
+      <c r="F39" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="G39" s="2">
+        <f>B39*F39</f>
+        <v>0.38</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>2</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="G43" s="2">
+        <f>B43*F43</f>
+        <v>0.16</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="G41" s="2">
-        <f>B41*F41</f>
-        <v>0.16</v>
-      </c>
-      <c r="H41" s="1" t="s">
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G44" s="2">
+        <f>B44*F44</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G42" s="2">
-        <f>B42*F42</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C44" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G44" s="2">
-        <f>SUM(F3:F42)</f>
-        <v>234.26999999999998</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="9" t="s">
+    <row r="46" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C46" s="8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="9"/>
+      <c r="G46" s="2">
+        <f>SUM(F3:F44)</f>
+        <v>259.16999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1"/>
     <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H5" r:id="rId3" display="https://www.zyltech.com/2040-v-groove-extrusion-pre-cut-lengths-300mm-2000mm/?sku=EXT-2040-REG-300-VGRV"/>
-    <hyperlink ref="H6" r:id="rId4" display="https://www.zyltech.com/2040-v-groove-extrusion-pre-cut-lengths-300mm-2000mm/?sku=EXT-2040-REG-300-VGRV"/>
-    <hyperlink ref="H8" r:id="rId5"/>
-    <hyperlink ref="H10" r:id="rId6"/>
-    <hyperlink ref="H12" r:id="rId7"/>
-    <hyperlink ref="H13" r:id="rId8"/>
-    <hyperlink ref="H14" r:id="rId9"/>
-    <hyperlink ref="H22" r:id="rId10"/>
-    <hyperlink ref="H20" r:id="rId11"/>
-    <hyperlink ref="H29" r:id="rId12"/>
-    <hyperlink ref="H30" r:id="rId13"/>
-    <hyperlink ref="H31" r:id="rId14"/>
-    <hyperlink ref="H32" r:id="rId15"/>
-    <hyperlink ref="H34" r:id="rId16"/>
-    <hyperlink ref="H35" r:id="rId17"/>
-    <hyperlink ref="H36" r:id="rId18"/>
-    <hyperlink ref="H37" r:id="rId19"/>
-    <hyperlink ref="H41" r:id="rId20"/>
-    <hyperlink ref="H42" r:id="rId21"/>
-    <hyperlink ref="H19" r:id="rId22"/>
-    <hyperlink ref="H15" r:id="rId23"/>
-    <hyperlink ref="H16" r:id="rId24"/>
-    <hyperlink ref="H17" r:id="rId25"/>
-    <hyperlink ref="H18" r:id="rId26"/>
-    <hyperlink ref="H23" r:id="rId27"/>
-    <hyperlink ref="H11" r:id="rId28"/>
-    <hyperlink ref="H7" r:id="rId29"/>
+    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="H10" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H14" r:id="rId7"/>
+    <hyperlink ref="H15" r:id="rId8"/>
+    <hyperlink ref="H16" r:id="rId9"/>
+    <hyperlink ref="H24" r:id="rId10"/>
+    <hyperlink ref="H22" r:id="rId11"/>
+    <hyperlink ref="H31" r:id="rId12"/>
+    <hyperlink ref="H32" r:id="rId13"/>
+    <hyperlink ref="H33" r:id="rId14"/>
+    <hyperlink ref="H34" r:id="rId15"/>
+    <hyperlink ref="H36" r:id="rId16"/>
+    <hyperlink ref="H37" r:id="rId17"/>
+    <hyperlink ref="H38" r:id="rId18"/>
+    <hyperlink ref="H39" r:id="rId19"/>
+    <hyperlink ref="H43" r:id="rId20"/>
+    <hyperlink ref="H44" r:id="rId21"/>
+    <hyperlink ref="H21" r:id="rId22"/>
+    <hyperlink ref="H17" r:id="rId23"/>
+    <hyperlink ref="H18" r:id="rId24"/>
+    <hyperlink ref="H19" r:id="rId25"/>
+    <hyperlink ref="H20" r:id="rId26"/>
+    <hyperlink ref="H25" r:id="rId27"/>
+    <hyperlink ref="H13" r:id="rId28"/>
+    <hyperlink ref="H8" r:id="rId29"/>
+    <hyperlink ref="H9" r:id="rId30"/>
+    <hyperlink ref="H7" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId30"/>
+  <pageSetup orientation="landscape" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>